<commit_message>
EPBDS-12787 No bruteforce implementation.
</commit_message>
<xml_diff>
--- a/ITEST/itest.WebService-lazy/openl-repository/EPBDS-10699/EPBDS-10699/Main-auto.xlsx
+++ b/ITEST/itest.WebService-lazy/openl-repository/EPBDS-10699/EPBDS-10699/Main-auto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ymolchan\Desktop\www2-DEFAULT-2020-11-11_11-10-19\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\openl-tablets\ITEST\itest.WebService-lazy\openl-repository\EPBDS-10699\EPBDS-10699\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E9F189-FC3E-4316-852E-CB80A3410E6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9030659C-E3CB-482A-8437-544E67A78541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35085" yWindow="3570" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4410" yWindow="990" windowWidth="27840" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
     <t>RETURN</t>
   </si>
   <si>
-    <t>= addAll(null, null); "Hello";</t>
+    <t>= addAll1(null, null); "Hello";</t>
   </si>
 </sst>
 </file>
@@ -78,11 +78,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -363,41 +364,41 @@
   <dimension ref="B3:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B8"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>